<commit_message>
sorting kassabuch in invoicenumber before saving
</commit_message>
<xml_diff>
--- a/Vorlagen/Vorlage_LandTirol_Brigitte.xlsx
+++ b/Vorlagen/Vorlage_LandTirol_Brigitte.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brigittemacbookpro/Brigitte Aron/Rechnung__Logopädie/Abrechnungsprogramm Leander/Vorlagen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{869CAF5F-C6CD-DF47-AAD8-18F9F9D997B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3027E53-1095-F24C-82FE-89AA5497CA22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Rechnung Einrichtung" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Rechnung Einrichtung'!$A$1:$H$56</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Rechnung Einrichtung'!$A$1:$G$53</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -101,9 +101,6 @@
     <t>Stundensatz (60 Min)</t>
   </si>
   <si>
-    <t>Anzahl Hausbesuche</t>
-  </si>
-  <si>
     <t>Summe</t>
   </si>
   <si>
@@ -147,6 +144,9 @@
   </si>
   <si>
     <t>Innsbruck, am:</t>
+  </si>
+  <si>
+    <t>Hausbesuch</t>
   </si>
 </sst>
 </file>
@@ -405,14 +405,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" shrinkToFit="1"/>
     </xf>
@@ -467,6 +461,25 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -476,27 +489,8 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -834,567 +828,563 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5:H17"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A19" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="24.83203125" customWidth="1"/>
-    <col min="2" max="2" width="8.83203125" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
     <col min="4" max="4" width="7.1640625" customWidth="1"/>
     <col min="5" max="5" width="11.1640625" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" customWidth="1"/>
-    <col min="7" max="7" width="9" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A3" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B3" s="31" t="s">
         <v>32</v>
-      </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A3" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="39" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="36"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="4"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="5"/>
+      <c r="C5" s="3"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="38"/>
-      <c r="C7" s="4" t="s">
+      <c r="B7" s="41"/>
+      <c r="C7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="4"/>
+      <c r="D7" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="32"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="D15" s="42" t="s">
+      <c r="D15" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="35"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="6"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="D16" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="33"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="32"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="B18" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+    </row>
+    <row r="20" spans="1:7" ht="42" x14ac:dyDescent="0.15">
+      <c r="A20" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="42"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="8"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="D16" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="E16" s="43"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="41"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B18" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31"/>
-    </row>
-    <row r="20" spans="1:7" ht="42" x14ac:dyDescent="0.15">
-      <c r="A20" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F20" s="10" t="s">
+      <c r="G20" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="G20" s="11" t="s">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A21" s="10"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="13">
+        <v>76.03</v>
+      </c>
+      <c r="F21" s="12"/>
+      <c r="G21" s="14">
+        <f>D21*E21</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A22" s="15"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13">
+        <v>29</v>
+      </c>
+      <c r="G22" s="14">
+        <f>D22*F22</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A23" s="16"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="40" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A21" s="12"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="15">
-        <v>74.2</v>
-      </c>
-      <c r="F21" s="14"/>
-      <c r="G21" s="16">
-        <f>D21*E21</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A22" s="17"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15">
+      <c r="E23" s="40"/>
+      <c r="F23" s="18">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="G23" s="19">
+        <f>(G21+G22)*0.034</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A24" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="39"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="20">
+        <f>SUM(G21:G23)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A25" s="21"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="22"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A26" s="10"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="13">
+        <v>76.03</v>
+      </c>
+      <c r="F26" s="12"/>
+      <c r="G26" s="14">
+        <f>D26*E26</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A27" s="15"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13">
         <v>29</v>
       </c>
-      <c r="G22" s="16">
-        <f>F21*F22</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A23" s="18"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="E23" s="35"/>
-      <c r="F23" s="20">
+      <c r="G27" s="14">
+        <f>D27*F27</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A28" s="16"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" s="40"/>
+      <c r="F28" s="18">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="G23" s="21">
-        <f>G21*0.034</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A24" s="34" t="s">
+      <c r="G28" s="19">
+        <f>(G26+G27)*0.034</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A29" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="34"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="22">
-        <f>SUM(G21:G23)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A25" s="23"/>
-      <c r="B25" s="23"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="24"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A26" s="12"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="15">
-        <v>74.2</v>
-      </c>
-      <c r="F26" s="14"/>
-      <c r="G26" s="16">
-        <f>D26*E26</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A27" s="17"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15">
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="20">
+        <f>SUM(G26:G28)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A30" s="23"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="22"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A31" s="10"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="13">
+        <v>76.03</v>
+      </c>
+      <c r="F31" s="12"/>
+      <c r="G31" s="14">
+        <f>D31*E31</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A32" s="10"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="13">
         <v>29</v>
       </c>
-      <c r="G27" s="16">
-        <f>F26*F27</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A28" s="18"/>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="E28" s="35"/>
-      <c r="F28" s="20">
+      <c r="G32" s="14">
+        <f>D32*F32</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A33" s="16"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E33" s="12"/>
+      <c r="F33" s="25">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="G28" s="21">
-        <f>G26*0.034</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A29" s="34" t="s">
+      <c r="G33" s="19">
+        <f>(G31+G32)*0.034</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A34" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="34"/>
-      <c r="C29" s="34"/>
-      <c r="D29" s="34"/>
-      <c r="E29" s="34"/>
-      <c r="F29" s="34"/>
-      <c r="G29" s="22">
-        <f>SUM(G26:G28)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A30" s="25"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="24"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A31" s="12"/>
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="15">
-        <v>74.2</v>
-      </c>
-      <c r="F31" s="14"/>
-      <c r="G31" s="16">
-        <f>D31*E31</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A32" s="12"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="15">
+      <c r="B34" s="39"/>
+      <c r="C34" s="39"/>
+      <c r="D34" s="39"/>
+      <c r="E34" s="39"/>
+      <c r="F34" s="39"/>
+      <c r="G34" s="20">
+        <f>SUM(G31:G33)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A35" s="23"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="22"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A36" s="15"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="13">
+        <v>76.03</v>
+      </c>
+      <c r="F36" s="12"/>
+      <c r="G36" s="14">
+        <f>D36*E36</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A37" s="15"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13">
         <v>29</v>
       </c>
-      <c r="G32" s="16">
-        <f>F31*F32</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A33" s="18"/>
-      <c r="B33" s="19"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="E33" s="14"/>
-      <c r="F33" s="27">
+      <c r="G37" s="14">
+        <f>D37*F37</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A38" s="16"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="E38" s="40"/>
+      <c r="F38" s="18">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="G33" s="21">
-        <f>G31*0.034</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A34" s="34" t="s">
+      <c r="G38" s="19">
+        <f>(G36+G37)*0.034</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A39" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="B34" s="34"/>
-      <c r="C34" s="34"/>
-      <c r="D34" s="34"/>
-      <c r="E34" s="34"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="22">
-        <f>SUM(G31:G33)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A35" s="25"/>
-      <c r="E35" s="26"/>
-      <c r="F35" s="26"/>
-      <c r="G35" s="24"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A36" s="17"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="15">
-        <v>74.2</v>
-      </c>
-      <c r="F36" s="14"/>
-      <c r="G36" s="16">
-        <f>D36*E36</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A37" s="17"/>
-      <c r="B37" s="14"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="15"/>
-      <c r="F37" s="15">
+      <c r="B39" s="39"/>
+      <c r="C39" s="39"/>
+      <c r="D39" s="39"/>
+      <c r="E39" s="39"/>
+      <c r="F39" s="39"/>
+      <c r="G39" s="20">
+        <f>SUM(G36:G38)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A40" s="3"/>
+      <c r="B40" s="26"/>
+      <c r="C40" s="26"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="22"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A41" s="10"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="13">
+        <v>76.03</v>
+      </c>
+      <c r="F41" s="12"/>
+      <c r="G41" s="14">
+        <f>D41*E41</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A42" s="15"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13">
         <v>29</v>
       </c>
-      <c r="G37" s="16">
-        <f>F36*F37</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A38" s="18"/>
-      <c r="B38" s="19"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="E38" s="35"/>
-      <c r="F38" s="20">
+      <c r="G42" s="14">
+        <f>D42*F42</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A43" s="16"/>
+      <c r="B43" s="17"/>
+      <c r="C43" s="17"/>
+      <c r="D43" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="E43" s="40"/>
+      <c r="F43" s="18">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="G38" s="21">
-        <f>G36*0.034</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A39" s="34" t="s">
+      <c r="G43" s="19">
+        <f>(G41+G42)*0.034</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A44" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="B39" s="34"/>
-      <c r="C39" s="34"/>
-      <c r="D39" s="34"/>
-      <c r="E39" s="34"/>
-      <c r="F39" s="34"/>
-      <c r="G39" s="22">
-        <f>SUM(G36:G38)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A40" s="5"/>
-      <c r="B40" s="28"/>
-      <c r="C40" s="28"/>
-      <c r="D40" s="23"/>
-      <c r="E40" s="23"/>
-      <c r="F40" s="23"/>
-      <c r="G40" s="24"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A41" s="12"/>
-      <c r="B41" s="13"/>
-      <c r="C41" s="13"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="15">
-        <v>74.2</v>
-      </c>
-      <c r="F41" s="14"/>
-      <c r="G41" s="16">
-        <f>D41*E41</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A42" s="17"/>
-      <c r="B42" s="14"/>
-      <c r="C42" s="14"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="15"/>
-      <c r="F42" s="15">
-        <v>29</v>
-      </c>
-      <c r="G42" s="16">
-        <f>F41*F42</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A43" s="18"/>
-      <c r="B43" s="19"/>
-      <c r="C43" s="19"/>
-      <c r="D43" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="E43" s="35"/>
-      <c r="F43" s="20">
-        <v>3.4000000000000002E-2</v>
-      </c>
-      <c r="G43" s="21">
-        <f>G41*0.034</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A44" s="34" t="s">
+      <c r="B44" s="39"/>
+      <c r="C44" s="39"/>
+      <c r="D44" s="39"/>
+      <c r="E44" s="39"/>
+      <c r="F44" s="39"/>
+      <c r="G44" s="20">
+        <f>SUM(G41:G43)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A45" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="B44" s="34"/>
-      <c r="C44" s="34"/>
-      <c r="D44" s="34"/>
-      <c r="E44" s="34"/>
-      <c r="F44" s="34"/>
-      <c r="G44" s="22">
-        <f>SUM(G41:G43)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A45" s="33" t="s">
+      <c r="B45" s="38"/>
+      <c r="C45" s="38"/>
+      <c r="D45" s="38"/>
+      <c r="E45" s="38"/>
+      <c r="F45" s="38"/>
+      <c r="G45" s="27">
+        <f>SUM(G24,G29,G34,G39,G44)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="E46" s="24"/>
+      <c r="F46" s="24"/>
+      <c r="G46" s="24"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A47" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B45" s="33"/>
-      <c r="C45" s="33"/>
-      <c r="D45" s="33"/>
-      <c r="E45" s="33"/>
-      <c r="F45" s="33"/>
-      <c r="G45" s="29">
-        <f>SUM(G24,G29,G34,G39,G44)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="E46" s="26"/>
-      <c r="F46" s="26"/>
-      <c r="G46" s="26"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A47" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E47" s="26"/>
-      <c r="F47" s="26"/>
-      <c r="G47" s="26"/>
+      <c r="E47" s="24"/>
+      <c r="F47" s="24"/>
+      <c r="G47" s="24"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A48" s="5"/>
-      <c r="B48" s="5"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
-      <c r="F48" s="5"/>
-      <c r="G48" s="30"/>
+      <c r="A48" s="3"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="28"/>
     </row>
     <row r="49" spans="5:7" x14ac:dyDescent="0.15">
-      <c r="E49" s="26"/>
-      <c r="F49" s="26"/>
-      <c r="G49" s="26"/>
+      <c r="E49" s="24"/>
+      <c r="F49" s="24"/>
+      <c r="G49" s="24"/>
     </row>
     <row r="50" spans="5:7" x14ac:dyDescent="0.15">
-      <c r="E50" s="26"/>
-      <c r="F50" s="26"/>
-      <c r="G50" s="26"/>
+      <c r="E50" s="24"/>
+      <c r="F50" s="24"/>
+      <c r="G50" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B4:C4"/>
+  <mergeCells count="11">
     <mergeCell ref="A7:B7"/>
-    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="A24:F24"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="A29:F29"/>
     <mergeCell ref="A45:F45"/>
     <mergeCell ref="A34:F34"/>
     <mergeCell ref="D38:E38"/>
     <mergeCell ref="A39:F39"/>
     <mergeCell ref="D43:E43"/>
     <mergeCell ref="A44:F44"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="A24:F24"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="A29:F29"/>
   </mergeCells>
   <pageMargins left="1.0208333333333299" right="0.25" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
-    <oddFooter>&amp;Lx Gemäß § 6 UStG i.d.g.F. befreit
-Zutreffendes bitte ankreuzen</oddFooter>
+    <oddFooter xml:space="preserve">&amp;L&amp;K000000Gemäß § 6 UStG i.d.g.F. befreit
+</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>